<commit_message>
Se actualizó el calendario con el inicio y terminacion de cada actividad
</commit_message>
<xml_diff>
--- a/Documentacion/Calendario.xlsx
+++ b/Documentacion/Calendario.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>Etapas</t>
   </si>
@@ -41,13 +41,22 @@
     <t>Backend</t>
   </si>
   <si>
-    <t>Frondend</t>
-  </si>
-  <si>
     <t>Pruebas</t>
   </si>
   <si>
     <t>Documentacion</t>
+  </si>
+  <si>
+    <t>Inicia</t>
+  </si>
+  <si>
+    <t>Termina</t>
+  </si>
+  <si>
+    <t>Frontend</t>
+  </si>
+  <si>
+    <t>OK</t>
   </si>
 </sst>
 </file>
@@ -88,15 +97,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -119,11 +134,123 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -135,9 +262,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -145,17 +269,86 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C6" sqref="C6:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,216 +643,238 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-    </row>
-    <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="34"/>
+    </row>
+    <row r="2" spans="1:14" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
+      <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="28"/>
+    </row>
+    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B3" s="6">
         <v>42191</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C3" s="6">
         <v>42192</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D3" s="6">
         <v>42193</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E3" s="6">
         <v>42194</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F3" s="6">
         <v>42195</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G3" s="6">
         <v>42196</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H3" s="6">
         <v>42197</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I3" s="6">
         <v>42198</v>
       </c>
-      <c r="J2" s="7">
+      <c r="J3" s="6">
         <v>42199</v>
       </c>
-      <c r="K2" s="8">
+      <c r="K3" s="7">
         <v>42200</v>
       </c>
-      <c r="L2" s="7">
+      <c r="L3" s="6">
         <v>42201</v>
       </c>
-      <c r="M2" s="7">
+      <c r="M3" s="6">
         <v>42202</v>
       </c>
-      <c r="N2" s="9"/>
-    </row>
-    <row r="3" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="N3" s="35"/>
+    </row>
+    <row r="4" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="13"/>
-    </row>
-    <row r="4" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="B4" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="39"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="36"/>
+    </row>
+    <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="37"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="36"/>
+    </row>
+    <row r="6" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="13"/>
-    </row>
-    <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="13"/>
-    </row>
-    <row r="6" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
       <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="13"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="36"/>
     </row>
     <row r="7" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
+      <c r="A7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="22"/>
+      <c r="C7" s="10"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="13"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="36"/>
+    </row>
+    <row r="8" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="24"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="K8" s="16"/>
+      <c r="L8" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="M8" s="30"/>
+      <c r="N8" s="36"/>
+    </row>
+    <row r="9" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="25"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="36"/>
+    </row>
+    <row r="10" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+      <c r="B10" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="M10" s="30"/>
+      <c r="N10" s="36"/>
+    </row>
+    <row r="11" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="36"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
@@ -736,14 +951,78 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B1:N1"/>
+  <mergeCells count="7">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B11:L11"/>
+    <mergeCell ref="B1:M1"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="J9:L9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Se actualizo el documento calendario
</commit_message>
<xml_diff>
--- a/Documentacion/Calendario.xlsx
+++ b/Documentacion/Calendario.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Etapas</t>
   </si>
@@ -57,6 +57,24 @@
   </si>
   <si>
     <t>OK</t>
+  </si>
+  <si>
+    <t>Responsable</t>
+  </si>
+  <si>
+    <t>Alejandro de Jesus Zazueta Peñuelas</t>
+  </si>
+  <si>
+    <t>Jorge Luis Lopez Payan</t>
+  </si>
+  <si>
+    <t>Manuel Alejandro Verdugo Perez</t>
+  </si>
+  <si>
+    <t>Victor Alain Torrecillas Camacho y Hector Eduardo Garcia Mata</t>
+  </si>
+  <si>
+    <t>Juan Pablo Bracamontes Astorga y Alejandro de Jesus Zazueta Peñuelas</t>
   </si>
 </sst>
 </file>
@@ -111,7 +129,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -237,20 +255,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -259,16 +268,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -278,21 +280,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -303,10 +290,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -315,17 +298,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -343,11 +321,56 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -632,249 +655,262 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:J6"/>
+      <selection activeCell="B11" sqref="B11:L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1"/>
-    <col min="2" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="34"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="21"/>
     </row>
     <row r="2" spans="1:14" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="26"/>
+      <c r="B2" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="28"/>
-    </row>
-    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="18"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="17"/>
+    </row>
+    <row r="3" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="36">
         <v>42191</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="36">
         <v>42192</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="40">
         <v>42193</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="40">
         <v>42194</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="40">
         <v>42195</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="40">
         <v>42196</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="40">
         <v>42197</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="40">
         <v>42198</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="40">
         <v>42199</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="41">
         <v>42200</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="40">
         <v>42201</v>
       </c>
-      <c r="M3" s="6">
-        <v>42202</v>
-      </c>
-      <c r="N3" s="35"/>
-    </row>
-    <row r="4" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="M3" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" s="22"/>
+    </row>
+    <row r="4" spans="1:14" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="36"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4" s="23"/>
     </row>
     <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="37"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="17" t="s">
+      <c r="A5" s="24"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="18" t="s">
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="22"/>
-      <c r="L5" s="22"/>
-      <c r="M5" s="30"/>
-      <c r="N5" s="36"/>
-    </row>
-    <row r="6" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="23"/>
+    </row>
+    <row r="6" spans="1:14" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="36"/>
-    </row>
-    <row r="7" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="B6" s="12"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="N6" s="23"/>
+    </row>
+    <row r="7" spans="1:14" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="36"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N7" s="23"/>
     </row>
     <row r="8" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="17" t="s">
+      <c r="A8" s="14"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="16"/>
-      <c r="L8" s="20" t="s">
+      <c r="K8" s="8"/>
+      <c r="L8" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="M8" s="30"/>
-      <c r="N8" s="36"/>
-    </row>
-    <row r="9" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="M8" s="5"/>
+      <c r="N8" s="23"/>
+    </row>
+    <row r="9" spans="1:14" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="36"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="N9" s="23"/>
     </row>
     <row r="10" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="17" t="s">
+      <c r="A10" s="7"/>
+      <c r="B10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="20" t="s">
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="M10" s="30"/>
-      <c r="N10" s="36"/>
-    </row>
-    <row r="11" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="M10" s="5"/>
+      <c r="N10" s="23"/>
+    </row>
+    <row r="11" spans="1:14" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="36"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="N11" s="23"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>

</xml_diff>

<commit_message>
Se actualizo el calendario
</commit_message>
<xml_diff>
--- a/Documentacion/Calendario.xlsx
+++ b/Documentacion/Calendario.xlsx
@@ -115,7 +115,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,6 +125,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -259,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -321,57 +333,55 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -655,7 +665,8 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:L11"/>
+      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,31 +680,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="39"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="35"/>
       <c r="N1" s="21"/>
     </row>
     <row r="2" spans="1:14" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="35" t="s">
+      <c r="A2" s="31"/>
+      <c r="B2" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="27" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="18"/>
@@ -712,40 +723,40 @@
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="36">
+      <c r="B3" s="26">
         <v>42191</v>
       </c>
-      <c r="C3" s="36">
+      <c r="C3" s="26">
         <v>42192</v>
       </c>
-      <c r="D3" s="40">
+      <c r="D3" s="28">
         <v>42193</v>
       </c>
-      <c r="E3" s="40">
+      <c r="E3" s="28">
         <v>42194</v>
       </c>
-      <c r="F3" s="40">
+      <c r="F3" s="28">
         <v>42195</v>
       </c>
-      <c r="G3" s="40">
+      <c r="G3" s="28">
         <v>42196</v>
       </c>
-      <c r="H3" s="40">
+      <c r="H3" s="28">
         <v>42197</v>
       </c>
-      <c r="I3" s="40">
+      <c r="I3" s="28">
         <v>42198</v>
       </c>
-      <c r="J3" s="40">
+      <c r="J3" s="28">
         <v>42199</v>
       </c>
-      <c r="K3" s="41">
+      <c r="K3" s="29">
         <v>42200</v>
       </c>
-      <c r="L3" s="40">
+      <c r="L3" s="28">
         <v>42201</v>
       </c>
-      <c r="M3" s="40" t="s">
+      <c r="M3" s="28" t="s">
         <v>11</v>
       </c>
       <c r="N3" s="22"/>
@@ -754,10 +765,10 @@
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="33"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
@@ -797,14 +808,14 @@
         <v>4</v>
       </c>
       <c r="B6" s="12"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="29"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
       <c r="M6" s="5" t="s">
@@ -817,14 +828,14 @@
         <v>9</v>
       </c>
       <c r="B7" s="12"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="34"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="41"/>
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
       <c r="M7" s="5" t="s">
@@ -864,9 +875,9 @@
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="39"/>
       <c r="M9" s="5" t="s">
         <v>15</v>
       </c>
@@ -892,21 +903,21 @@
       <c r="M10" s="5"/>
       <c r="N10" s="23"/>
     </row>
-    <row r="11" spans="1:14" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="28"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="40"/>
+      <c r="L11" s="39"/>
       <c r="M11" s="5" t="s">
         <v>16</v>
       </c>
@@ -1051,14 +1062,10 @@
       <c r="A21" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="3">
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B11:L11"/>
     <mergeCell ref="B1:M1"/>
     <mergeCell ref="B4:C4"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="J9:L9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>